<commit_message>
Pdf de las historias de usuario
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACION/1.3 HIstorias de Usuario/GN_Matriz de Marco de Trabajo HU V1.1.xlsx
+++ b/PREGAME/1. ELICITACION/1.3 HIstorias de Usuario/GN_Matriz de Marco de Trabajo HU V1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uespe-my.sharepoint.com/personal/dgreinoso_espe_edu_ec/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\6TO SEMESTRE\ANALISIS Y DISEÑO DE SOFTWARE\REPOSITORIO\22426_G2_ADS\PREGAME\1. ELICITACION\1.3 HIstorias de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F60BEAB8-E414-41BB-9997-1ED7FEC35B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E05397-D8CD-4D62-8CEE-BDA93EA64026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId1"/>
@@ -877,16 +877,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -913,30 +922,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -954,6 +956,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -979,25 +987,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,31 +1336,31 @@
   </sheetPr>
   <dimension ref="B1:O1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="15" customWidth="1"/>
-    <col min="3" max="5" width="20.625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="13.125" style="15" customWidth="1"/>
+    <col min="1" max="1" width="4.59765625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="6.59765625" style="15" customWidth="1"/>
+    <col min="3" max="5" width="20.59765625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" style="15" customWidth="1"/>
     <col min="7" max="7" width="32.5" style="15" customWidth="1"/>
-    <col min="8" max="12" width="10.625" style="15" customWidth="1"/>
-    <col min="13" max="13" width="32.75" style="15" customWidth="1"/>
-    <col min="14" max="15" width="20.625" style="15" customWidth="1"/>
-    <col min="16" max="26" width="9.375" style="15" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="15"/>
+    <col min="8" max="12" width="10.59765625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="32.69921875" style="15" customWidth="1"/>
+    <col min="14" max="15" width="20.59765625" style="15" customWidth="1"/>
+    <col min="16" max="26" width="9.3984375" style="15" customWidth="1"/>
+    <col min="27" max="16384" width="12.59765625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="16.5">
+    <row r="1" spans="2:15" ht="13.8">
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
       <c r="K1" s="17"/>
       <c r="L1" s="16"/>
     </row>
-    <row r="2" spans="2:15" ht="16.5">
+    <row r="2" spans="2:15" ht="13.8">
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="K2" s="17"/>
@@ -1370,21 +1370,21 @@
       <c r="B3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="79"/>
-    </row>
-    <row r="4" spans="2:15" ht="16.5">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="45"/>
+    </row>
+    <row r="4" spans="2:15" ht="13.8">
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="17"/>
@@ -7826,7 +7826,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.55118110236220474" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="40" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7837,51 +7837,51 @@
   </sheetPr>
   <dimension ref="B2:P1020"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.375" customWidth="1"/>
-    <col min="2" max="2" width="2.625" customWidth="1"/>
-    <col min="3" max="15" width="10.625" customWidth="1"/>
-    <col min="16" max="16" width="2.625" customWidth="1"/>
-    <col min="17" max="26" width="9.375" customWidth="1"/>
+    <col min="1" max="1" width="9.3984375" customWidth="1"/>
+    <col min="2" max="2" width="2.59765625" customWidth="1"/>
+    <col min="3" max="15" width="10.59765625" customWidth="1"/>
+    <col min="16" max="16" width="2.59765625" customWidth="1"/>
+    <col min="17" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="15" hidden="1" customHeight="1"/>
     <row r="3" spans="2:16" ht="15" hidden="1" customHeight="1"/>
-    <row r="4" spans="2:16" hidden="1">
+    <row r="4" spans="2:16" ht="14.4" hidden="1">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:16" hidden="1">
+    <row r="5" spans="2:16" ht="14.4" hidden="1">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1">
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="67"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1">
       <c r="C7" s="3"/>
@@ -7921,15 +7921,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="81"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -7944,17 +7944,17 @@
         <v>83</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="58" t="str">
+      <c r="E10" s="69" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,5,0)</f>
         <v>Propietario</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="58" t="str">
+      <c r="H10" s="69" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,11,0)</f>
         <v>No iniciado</v>
       </c>
-      <c r="I10" s="81"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="9"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -7986,15 +7986,15 @@
         <v>95</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="81"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="I12" s="81"/>
+      <c r="I12" s="67"/>
       <c r="J12" s="9"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -8010,17 +8010,17 @@
         <v>3</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="58" t="str">
+      <c r="E13" s="69" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="81"/>
+      <c r="F13" s="67"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="58" t="str">
+      <c r="H13" s="69" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,7,0)</f>
         <v>Gabriel Reinoso</v>
       </c>
-      <c r="I13" s="81"/>
+      <c r="I13" s="67"/>
       <c r="J13" s="9"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
@@ -8048,68 +8048,68 @@
     </row>
     <row r="15" spans="2:16" ht="19.5" customHeight="1">
       <c r="B15" s="38"/>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="64" t="str">
+      <c r="D15" s="74" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,3,0)</f>
         <v>El sistema deberá permitir que el propietario  pueda generar  un reporte de una materia prima en especifico</v>
       </c>
-      <c r="E15" s="65"/>
+      <c r="E15" s="75"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="64" t="str">
+      <c r="H15" s="74" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,4,0)</f>
         <v>Para que tenga una visión clara del inventario durante una materia prima especifica</v>
       </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="83"/>
       <c r="K15" s="30"/>
-      <c r="L15" s="44" t="s">
+      <c r="L15" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="M15" s="47" t="str">
+      <c r="M15" s="90" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,6,0)</f>
         <v xml:space="preserve">El propietario selecciona  el nombre de la materia prima de la que quiere el reporte                                                                        El sistema genera el reporte </v>
       </c>
-      <c r="N15" s="48"/>
-      <c r="O15" s="49"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="58"/>
       <c r="P15" s="39"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1">
       <c r="B16" s="38"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="77"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="74"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="86"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="52"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="61"/>
       <c r="P16" s="39"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1">
       <c r="B17" s="38"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="79"/>
       <c r="F17" s="30"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="77"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="89"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="55"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="64"/>
       <c r="P17" s="39"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1">
@@ -8131,41 +8131,41 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1">
       <c r="B19" s="38"/>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="84"/>
-      <c r="E19" s="56" t="str">
+      <c r="D19" s="50"/>
+      <c r="E19" s="91" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,14,0)</f>
         <v xml:space="preserve">Generar reportes por Materia prima </v>
       </c>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="86"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
+      <c r="O19" s="93"/>
       <c r="P19" s="39"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1">
       <c r="B20" s="38"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="91"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="96"/>
       <c r="P20" s="39"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1">
@@ -8187,63 +8187,63 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1">
       <c r="B22" s="38"/>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="84"/>
-      <c r="E22" s="61" t="str">
+      <c r="D22" s="50"/>
+      <c r="E22" s="56" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,12,0)</f>
         <v>El aplicativo muestra el reporte de la materia prima seleccionada</v>
       </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="60" t="s">
+      <c r="J22" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="84"/>
-      <c r="L22" s="63" t="str">
+      <c r="K22" s="50"/>
+      <c r="L22" s="70" t="str">
         <f>VLOOKUP(C10,'Formato descripción HU'!B6:O19,13,0)</f>
         <v>N/A</v>
       </c>
-      <c r="M22" s="92"/>
-      <c r="N22" s="92"/>
-      <c r="O22" s="84"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="50"/>
       <c r="P22" s="39"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1">
       <c r="B23" s="38"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="52"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="93"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="93"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="94"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="55"/>
       <c r="P23" s="39"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1">
       <c r="B24" s="38"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="55"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="64"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="96"/>
-      <c r="N24" s="96"/>
-      <c r="O24" s="88"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="52"/>
       <c r="P24" s="39"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1">
@@ -9260,6 +9260,11 @@
     <row r="1020" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -9276,11 +9281,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -9316,11 +9316,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9519,22 +9520,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f1f31ffb-9912-4459-99c8-b26e82094b51" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64BB9B8E-F37C-4883-BB4F-987669CAAE30}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B92EABA-029D-4E15-9CAD-35D85D8AFEB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2E2F3D1-C235-4C14-B824-1A8C3F52885C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2E2F3D1-C235-4C14-B824-1A8C3F52885C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+    <ds:schemaRef ds:uri="ce621958-37b1-43fe-a1f1-1aad67996a88"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B92EABA-029D-4E15-9CAD-35D85D8AFEB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64BB9B8E-F37C-4883-BB4F-987669CAAE30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f1f31ffb-9912-4459-99c8-b26e82094b51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>